<commit_message>
Subject: some plitting changes
</commit_message>
<xml_diff>
--- a/Lab2/Lab2LocalThreads/threads_duration.xlsx
+++ b/Lab2/Lab2LocalThreads/threads_duration.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pancho\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Northeastern\CS6650 - Scalable Distributed Systems\Repos\CS6650-Distributed-System\lab2\Lab2LocalThreads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{E5D18E17-846E-41CB-AF99-ABDCD6CFA96C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE6C65D5-16CB-463E-BB7E-F2E6F9BF152C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="448" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja2" sheetId="3" r:id="rId1"/>
@@ -18,13 +18,13 @@
   </sheets>
   <calcPr calcId="0"/>
   <pivotCaches>
-    <pivotCache cacheId="16" r:id="rId3"/>
+    <pivotCache cacheId="0" r:id="rId3"/>
   </pivotCaches>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="18">
   <si>
     <t>task</t>
   </si>
@@ -83,7 +83,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
@@ -613,19 +613,7 @@
     <cellStyle name="Título 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="9">
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-    </dxf>
+  <dxfs count="5">
     <dxf>
       <numFmt numFmtId="164" formatCode="0.0"/>
     </dxf>
@@ -677,6 +665,9 @@
       <c:pivotFmt>
         <c:idx val="0"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -733,6 +724,9 @@
       <c:pivotFmt>
         <c:idx val="1"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -789,6 +783,9 @@
       <c:pivotFmt>
         <c:idx val="2"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -1096,6 +1093,9 @@
       <c:pivotFmt>
         <c:idx val="8"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -1109,6 +1109,174 @@
         </c:marker>
         <c:dLbl>
           <c:idx val="0"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="9"/>
+        <c:spPr>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="10"/>
+        <c:spPr>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="11"/>
+        <c:spPr>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -1135,7 +1303,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Collections1 - ArrayListSingleThread</c:v>
+                  <c:v>Collections2 - ConcurrentHashMapMultipleThreads</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1185,22 +1353,22 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>3</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>13</c:v>
+                  <c:v>98</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1221,7 +1389,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Collections1 - VectorSingleThread</c:v>
+                  <c:v>Collections2 - HashMapMultipleThreads</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1271,22 +1439,22 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>4</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>30</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1307,7 +1475,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Collections2 - ConcurrentHashMapMultipleThreads</c:v>
+                  <c:v>Collections2 - HashTableMultipleThreads</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1357,352 +1525,6 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>22</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>22</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>98</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-D446-4D61-8B55-3FBCF8F00F08}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Hoja2!$E$4:$E$6</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Collections2 - ConcurrentHashMapSingleThread</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:strRef>
-              <c:f>Hoja2!$A$7:$A$13</c:f>
-              <c:strCache>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1000</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>10000</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>100000</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1000000</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Hoja2!$E$7:$E$13</c:f>
-              <c:numCache>
-                <c:formatCode>0.0</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000004-D446-4D61-8B55-3FBCF8F00F08}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="4"/>
-          <c:order val="4"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Hoja2!$F$4:$F$6</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Collections2 - HashMapMultipleThreads</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent5"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:strRef>
-              <c:f>Hoja2!$A$7:$A$13</c:f>
-              <c:strCache>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1000</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>10000</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>100000</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1000000</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Hoja2!$F$7:$F$13</c:f>
-              <c:numCache>
-                <c:formatCode>0.0</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>19</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>19</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>58</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000005-D446-4D61-8B55-3FBCF8F00F08}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="5"/>
-          <c:order val="5"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Hoja2!$G$4:$G$6</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Collections2 - HashMapSingleThread</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent6"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:strRef>
-              <c:f>Hoja2!$A$7:$A$13</c:f>
-              <c:strCache>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1000</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>10000</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>100000</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1000000</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Hoja2!$G$7:$G$13</c:f>
-              <c:numCache>
-                <c:formatCode>0.0</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000006-D446-4D61-8B55-3FBCF8F00F08}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="6"/>
-          <c:order val="6"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Hoja2!$H$4:$H$6</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Collections2 - HashTableMultipleThreads</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1">
-                  <a:lumMod val="60000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:strRef>
-              <c:f>Hoja2!$A$7:$A$13</c:f>
-              <c:strCache>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1000</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>10000</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>100000</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1000000</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Hoja2!$H$7:$H$13</c:f>
-              <c:numCache>
-                <c:formatCode>0.0</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
                   <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="1">
@@ -1726,95 +1548,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000007-D446-4D61-8B55-3FBCF8F00F08}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="7"/>
-          <c:order val="7"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Hoja2!$I$4:$I$6</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Collections2 - HashTableSingleThread</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2">
-                  <a:lumMod val="60000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:strRef>
-              <c:f>Hoja2!$A$7:$A$13</c:f>
-              <c:strCache>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1000</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>10000</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>100000</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1000000</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Hoja2!$I$7:$I$13</c:f>
-              <c:numCache>
-                <c:formatCode>0.0</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>19</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000008-D446-4D61-8B55-3FBCF8F00F08}"/>
+              <c16:uniqueId val="{00000002-E801-4E9E-84C9-F38596ADEF3B}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2711,14 +2445,14 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>693965</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>121783</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>2081894</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>122464</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>1698173</xdr:colOff>
+      <xdr:colOff>1698174</xdr:colOff>
       <xdr:row>29</xdr:row>
       <xdr:rowOff>183697</xdr:rowOff>
     </xdr:to>
@@ -2749,7 +2483,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Pancho" refreshedDate="44593.939467824071" createdVersion="7" refreshedVersion="7" minRefreshableVersion="3" recordCount="54">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Pancho" refreshedDate="44593.939467824071" createdVersion="7" refreshedVersion="7" minRefreshableVersion="3" recordCount="54" xr:uid="{00000000-000A-0000-FFFF-FFFF10000000}">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:D55" sheet="out"/>
   </cacheSource>
@@ -3126,8 +2860,8 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TablaDinámica2" cacheId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="7" minRefreshableVersion="3" showDrill="0" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" compact="0" compactData="0" gridDropZones="1" multipleFieldFilters="0" chartFormat="4">
-  <location ref="A4:J13" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0000-000000000000}" name="TablaDinámica2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="7" minRefreshableVersion="3" showDrill="0" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" compact="0" compactData="0" gridDropZones="1" multipleFieldFilters="0" chartFormat="4">
+  <location ref="A4:E13" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
   <pivotFields count="4">
     <pivotField axis="axisCol" compact="0" outline="0" showAll="0" defaultSubtotal="0">
       <items count="3">
@@ -3143,15 +2877,15 @@
     </pivotField>
     <pivotField axis="axisCol" compact="0" outline="0" showAll="0" defaultSubtotal="0">
       <items count="9">
-        <item x="2"/>
+        <item h="1" x="2"/>
         <item x="8"/>
-        <item x="5"/>
+        <item h="1" x="5"/>
         <item x="7"/>
-        <item x="4"/>
+        <item h="1" x="4"/>
         <item x="6"/>
-        <item x="3"/>
+        <item h="1" x="3"/>
         <item h="1" x="0"/>
-        <item x="1"/>
+        <item h="1" x="1"/>
       </items>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
@@ -3202,32 +2936,16 @@
     <field x="0"/>
     <field x="1"/>
   </colFields>
-  <colItems count="9">
-    <i>
-      <x/>
-      <x/>
-    </i>
-    <i r="1">
-      <x v="8"/>
-    </i>
+  <colItems count="4">
     <i>
       <x v="1"/>
       <x v="1"/>
     </i>
     <i r="1">
-      <x v="2"/>
-    </i>
-    <i r="1">
       <x v="3"/>
     </i>
     <i r="1">
-      <x v="4"/>
-    </i>
-    <i r="1">
       <x v="5"/>
-    </i>
-    <i r="1">
-      <x v="6"/>
     </i>
     <i t="grand">
       <x/>
@@ -3237,11 +2955,11 @@
     <dataField name="Suma de durationMiliseconds" fld="3" baseField="0" baseItem="0" numFmtId="164"/>
   </dataFields>
   <formats count="1">
-    <format dxfId="8">
+    <format dxfId="4">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
   </formats>
-  <chartFormats count="9">
+  <chartFormats count="12">
     <chartFormat chart="3" format="0" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="1">
@@ -3361,6 +3079,51 @@
           </reference>
           <reference field="1" count="1" selected="0">
             <x v="7"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="3" format="9" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="3" format="10" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="8"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="3" format="11" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="1"/>
           </reference>
         </references>
       </pivotArea>
@@ -3674,21 +3437,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:J13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A4:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="9" width="34.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="34.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="9" width="34.42578125" bestFit="1" customWidth="1"/>
     <col min="10" max="11" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>17</v>
       </c>
@@ -3699,286 +3464,151 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D5" t="s">
         <v>7</v>
       </c>
       <c r="E5" t="s">
-        <v>7</v>
-      </c>
-      <c r="F5" t="s">
-        <v>7</v>
-      </c>
-      <c r="G5" t="s">
-        <v>7</v>
-      </c>
-      <c r="H5" t="s">
-        <v>7</v>
-      </c>
-      <c r="I5" t="s">
-        <v>7</v>
-      </c>
-      <c r="J5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="C6" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="D6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" t="s">
-        <v>12</v>
-      </c>
-      <c r="G6" t="s">
-        <v>9</v>
-      </c>
-      <c r="H6" t="s">
         <v>11</v>
       </c>
-      <c r="I6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>10</v>
       </c>
       <c r="B7" s="2">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="C7" s="2">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="D7" s="2">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E7" s="2">
-        <v>3</v>
-      </c>
-      <c r="F7" s="2">
-        <v>19</v>
-      </c>
-      <c r="G7" s="2">
-        <v>3</v>
-      </c>
-      <c r="H7" s="2">
-        <v>21</v>
-      </c>
-      <c r="I7" s="2">
-        <v>3</v>
-      </c>
-      <c r="J7" s="2">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>100</v>
       </c>
       <c r="B8" s="2">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="C8" s="2">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="D8" s="2">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E8" s="2">
-        <v>0</v>
-      </c>
-      <c r="F8" s="2">
-        <v>21</v>
-      </c>
-      <c r="G8" s="2">
-        <v>0</v>
-      </c>
-      <c r="H8" s="2">
-        <v>23</v>
-      </c>
-      <c r="I8" s="2">
-        <v>1</v>
-      </c>
-      <c r="J8" s="2">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1000</v>
       </c>
       <c r="B9" s="2">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="C9" s="2">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="D9" s="2">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E9" s="2">
-        <v>0</v>
-      </c>
-      <c r="F9" s="2">
-        <v>19</v>
-      </c>
-      <c r="G9" s="2">
-        <v>0</v>
-      </c>
-      <c r="H9" s="2">
-        <v>18</v>
-      </c>
-      <c r="I9" s="2">
-        <v>0</v>
-      </c>
-      <c r="J9" s="2">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>10000</v>
       </c>
       <c r="B10" s="2">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="C10" s="2">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="D10" s="2">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="E10" s="2">
-        <v>0</v>
-      </c>
-      <c r="F10" s="2">
-        <v>17</v>
-      </c>
-      <c r="G10" s="2">
-        <v>0</v>
-      </c>
-      <c r="H10" s="2">
-        <v>26</v>
-      </c>
-      <c r="I10" s="2">
-        <v>1</v>
-      </c>
-      <c r="J10" s="2">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>100000</v>
       </c>
       <c r="B11" s="2">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="C11" s="2">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="D11" s="2">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="E11" s="2">
-        <v>0</v>
-      </c>
-      <c r="F11" s="2">
-        <v>18</v>
-      </c>
-      <c r="G11" s="2">
-        <v>0</v>
-      </c>
-      <c r="H11" s="2">
-        <v>29</v>
-      </c>
-      <c r="I11" s="2">
-        <v>2</v>
-      </c>
-      <c r="J11" s="2">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1000000</v>
       </c>
       <c r="B12" s="2">
-        <v>13</v>
+        <v>98</v>
       </c>
       <c r="C12" s="2">
-        <v>30</v>
+        <v>58</v>
       </c>
       <c r="D12" s="2">
-        <v>98</v>
+        <v>65</v>
       </c>
       <c r="E12" s="2">
-        <v>0</v>
-      </c>
-      <c r="F12" s="2">
-        <v>58</v>
-      </c>
-      <c r="G12" s="2">
-        <v>1</v>
-      </c>
-      <c r="H12" s="2">
-        <v>65</v>
-      </c>
-      <c r="I12" s="2">
-        <v>19</v>
-      </c>
-      <c r="J12" s="2">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>14</v>
       </c>
       <c r="B13" s="2">
-        <v>20</v>
+        <v>195</v>
       </c>
       <c r="C13" s="2">
-        <v>37</v>
+        <v>152</v>
       </c>
       <c r="D13" s="2">
-        <v>195</v>
+        <v>182</v>
       </c>
       <c r="E13" s="2">
-        <v>3</v>
-      </c>
-      <c r="F13" s="2">
-        <v>152</v>
-      </c>
-      <c r="G13" s="2">
-        <v>4</v>
-      </c>
-      <c r="H13" s="2">
-        <v>182</v>
-      </c>
-      <c r="I13" s="2">
-        <v>26</v>
-      </c>
-      <c r="J13" s="2">
-        <v>619</v>
+        <v>529</v>
       </c>
     </row>
   </sheetData>
@@ -3988,7 +3618,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D55"/>
   <sheetViews>
     <sheetView topLeftCell="A34" workbookViewId="0"/>

</xml_diff>